<commit_message>
testNG upto excel to 2dArray
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunilkumarpatro/AutomationProjects/SelPractice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skpatro/sel/SelPractice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA106233-1A2A-1B47-8EBE-7B9D5847D35D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C97A12-4F46-DF42-A761-B6E82EBBD9F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13580" yWindow="3640" windowWidth="17300" windowHeight="12720" xr2:uid="{A7B795EB-10A4-8144-B6FD-389C14F815FC}"/>
+    <workbookView xWindow="40000" yWindow="3700" windowWidth="22700" windowHeight="14060" activeTab="1" xr2:uid="{A7B795EB-10A4-8144-B6FD-389C14F815FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>fullname</t>
   </si>
@@ -54,6 +55,36 @@
   </si>
   <si>
     <t>male</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>qwert2</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
   </si>
 </sst>
 </file>
@@ -419,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAA9555-1783-0146-8F82-D78890EC9D41}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -462,4 +493,68 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F6A3BB-E2FB-084D-B50C-627139B0D23D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>